<commit_message>
30 mismatch between doc and impl fix
</commit_message>
<xml_diff>
--- a/Documentation/F93M8_DocDb.xlsx
+++ b/Documentation/F93M8_DocDb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\FG9326M8GTEI4\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C057C20-884A-4A93-82A1-6914714D9087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E6EFDA-2C14-4536-B970-8701B0D928F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="847" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="266">
   <si>
     <t>Central Body Module</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Mass Erase Programming</t>
   </si>
   <si>
-    <t>Read Awake Reasons</t>
-  </si>
-  <si>
     <t>Read Coding Data</t>
   </si>
   <si>
@@ -198,12 +195,6 @@
   </si>
   <si>
     <t>RDBPI Climate Fan</t>
-  </si>
-  <si>
-    <t>RDBPI Air Quality Sensor</t>
-  </si>
-  <si>
-    <t>RDBPI Gas Sensor</t>
   </si>
   <si>
     <t>RDBPI Light Sensor</t>
@@ -774,58 +765,76 @@
     <t>DEC: Signal Invalid HC05 Connection Status</t>
   </si>
   <si>
-    <t>Gearbox in park
-Central locking activated.</t>
-  </si>
-  <si>
     <t>Gearbox in drive or in park
 Ignition switched to position two</t>
   </si>
   <si>
+    <t>HC05</t>
+  </si>
+  <si>
+    <t>HC05 Active</t>
+  </si>
+  <si>
+    <t>HC05 Ventilation</t>
+  </si>
+  <si>
+    <t>HC05 Ventilation Control</t>
+  </si>
+  <si>
+    <t>Stable distance</t>
+  </si>
+  <si>
+    <t>Time to collision warning time</t>
+  </si>
+  <si>
+    <t>Time to collision braking time</t>
+  </si>
+  <si>
+    <t>Maximum distance sensor</t>
+  </si>
+  <si>
+    <t>Minimum distance sensor</t>
+  </si>
+  <si>
+    <t>Invalid distance sensor</t>
+  </si>
+  <si>
+    <t>DEC: Message 0x001 DriveTrainStatus missing</t>
+  </si>
+  <si>
+    <t>CBM: Mcu Software Error</t>
+  </si>
+  <si>
+    <t>DMU: Mcu Software Error</t>
+  </si>
+  <si>
+    <t>CBM, DEC</t>
+  </si>
+  <si>
     <t>Gearbox in park
-Central locking de-activated</t>
-  </si>
-  <si>
-    <t>Gearbox in drive and vehicle speed greater than zero</t>
-  </si>
-  <si>
-    <t>HC05</t>
-  </si>
-  <si>
-    <t>HC05 Active</t>
-  </si>
-  <si>
-    <t>HC05 Ventilation</t>
-  </si>
-  <si>
-    <t>HC05 Ventilation Control</t>
-  </si>
-  <si>
-    <t>Stable distance</t>
-  </si>
-  <si>
-    <t>Time to collision warning time</t>
-  </si>
-  <si>
-    <t>Time to collision braking time</t>
-  </si>
-  <si>
-    <t>Maximum distance sensor</t>
-  </si>
-  <si>
-    <t>Minimum distance sensor</t>
-  </si>
-  <si>
-    <t>Invalid distance sensor</t>
-  </si>
-  <si>
-    <t>DEC: Message 0x001 DriveTrainStatus missing</t>
-  </si>
-  <si>
-    <t>CBM: Mcu Software Error</t>
-  </si>
-  <si>
-    <t>DMU: Mcu Software Error</t>
+Central locking activated.
+Ignition switched to position 0.</t>
+  </si>
+  <si>
+    <t>Gearbox in park
+Central locking de-activated.
+Ignition switched to position 0 or 1.</t>
+  </si>
+  <si>
+    <t>Gearbox in drive and vehicle speed greater than zero
+Ignition switched to position two.</t>
+  </si>
+  <si>
+    <t>Functionality</t>
+  </si>
+  <si>
+    <t>Transfer Data</t>
+  </si>
+  <si>
+    <t>Request Transfer Data</t>
+  </si>
+  <si>
+    <t>Transfer Exit</t>
   </si>
 </sst>
 </file>
@@ -987,7 +996,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1049,6 +1058,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1332,10 +1342,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,216 +1359,223 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="E1" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E2" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>147</v>
-      </c>
       <c r="F3" s="27" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>14</v>
-      </c>
       <c r="C5" s="12" t="s">
-        <v>16</v>
+        <v>158</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>250</v>
+        <v>146</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>162</v>
-      </c>
       <c r="E6" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>10</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>10</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>12</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>208</v>
+        <v>156</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>208</v>
+        <v>20</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1572,8 +1589,8 @@
   </sheetPr>
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,25 +1626,25 @@
         <v>26</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>24</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="P1" s="9" t="s">
         <v>24</v>
@@ -1638,37 +1655,37 @@
         <v>27</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J2" s="1">
         <v>2</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N2" s="1">
         <v>1</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1676,37 +1693,37 @@
         <v>28</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J3" s="1">
         <v>2</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N3" s="1">
         <v>1</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1714,37 +1731,37 @@
         <v>29</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G4" s="3">
         <v>28</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J4" s="1">
         <v>2</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N4" s="1">
         <v>100</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1752,37 +1769,37 @@
         <v>30</v>
       </c>
       <c r="B5" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="E5" s="24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G5" s="3">
         <v>32</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J5" s="1">
         <v>2</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N5" s="1">
         <v>20</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1790,37 +1807,37 @@
         <v>31</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G6" s="3">
         <v>33</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J6" s="1">
         <v>75</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N6" s="1">
         <v>255</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1828,37 +1845,37 @@
         <v>32</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G7" s="3">
         <v>34</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="J7" s="1">
         <v>4</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N7" s="1">
         <v>5</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1866,37 +1883,37 @@
         <v>33</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G8" s="3">
         <v>35</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J8" s="1">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N8" s="1">
         <v>15</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1904,37 +1921,37 @@
         <v>34</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="G9" s="3">
         <v>37</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J9" s="1">
         <v>1</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N9" s="1">
         <v>5</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1942,37 +1959,37 @@
         <v>35</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G10" s="3">
         <v>41</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J10" s="1">
         <v>1</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N10" s="1">
         <v>5</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1980,28 +1997,28 @@
         <v>36</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G11" s="3">
         <v>97</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="N11" s="1">
         <v>50</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2009,28 +2026,28 @@
         <v>37</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G12" s="3">
         <v>98</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="N12" s="1">
         <v>30</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2038,28 +2055,28 @@
         <v>38</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="G13" s="3">
         <v>99</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="N13" s="1">
         <v>15</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -2067,22 +2084,22 @@
         <v>39</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N14" s="1">
         <v>10</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -2090,22 +2107,22 @@
         <v>40</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N15" s="1">
         <v>80</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -2113,22 +2130,22 @@
         <v>41</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N16" s="1">
         <v>255</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2136,13 +2153,13 @@
         <v>42</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2150,13 +2167,13 @@
         <v>43</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2164,13 +2181,13 @@
         <v>44</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2178,13 +2195,13 @@
         <v>45</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2192,13 +2209,13 @@
         <v>46</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>63</v>
+        <v>258</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2206,13 +2223,13 @@
         <v>47</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>170</v>
+        <v>60</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2220,13 +2237,13 @@
         <v>48</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2234,13 +2251,13 @@
         <v>49</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2248,13 +2265,13 @@
         <v>50</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2262,13 +2279,13 @@
         <v>51</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2276,13 +2293,13 @@
         <v>52</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2290,13 +2307,13 @@
         <v>53</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2304,13 +2321,13 @@
         <v>54</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2318,13 +2335,13 @@
         <v>55</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2332,13 +2349,13 @@
         <v>56</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2346,13 +2363,13 @@
         <v>57</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2360,13 +2377,13 @@
         <v>58</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2374,55 +2391,55 @@
         <v>59</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>168</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>63</v>
+        <v>177</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>61</v>
+        <v>169</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>64</v>
+        <v>177</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>62</v>
+        <v>170</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>64</v>
+        <v>177</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2430,13 +2447,13 @@
         <v>171</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2444,13 +2461,13 @@
         <v>172</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2458,13 +2475,13 @@
         <v>173</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2472,13 +2489,13 @@
         <v>174</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E41" s="24" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2486,13 +2503,13 @@
         <v>175</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2500,95 +2517,95 @@
         <v>176</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>177</v>
+        <v>263</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>178</v>
+        <v>264</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>179</v>
+        <v>265</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D47" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E47" s="24" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D48" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D49" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="50" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D50" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="E50" s="24" t="s">
         <v>243</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D51" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E51" s="24" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -2605,7 +2622,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2620,7 +2637,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B1" s="21">
         <v>8</v>
@@ -2640,47 +2657,47 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>129</v>
-      </c>
       <c r="F2" s="19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>134</v>
-      </c>
       <c r="C3" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>135</v>
-      </c>
       <c r="F3" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B4" s="23">
         <v>475999</v>
@@ -2692,130 +2709,130 @@
         <v>300850</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>